<commit_message>
Temizlik ve ana fonksiyon güncellemeleri: gereksiz dosyalar silindi, yeni ve güncellenmiş dosyalar eklendi
</commit_message>
<xml_diff>
--- a/exports/test_scenarios_template.xlsx
+++ b/exports/test_scenarios_template.xlsx
@@ -593,17 +593,17 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>TC001</t>
+          <t>TC002</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Kullanıcı Girişi</t>
+          <t>Email Girişi</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Kullanıcının email ve şifre ile giriş yapabilmesi</t>
+          <t>Email alanına geçerli email adresi girilmesi</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="F3" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
@@ -651,17 +651,17 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>TC001</t>
+          <t>TC003</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Kullanıcı Girişi</t>
+          <t>Şifre Girişi</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Kullanıcının email ve şifre ile giriş yapabilmesi</t>
+          <t>Şifre alanına geçerli şifre girilmesi</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -675,11 +675,11 @@
         </is>
       </c>
       <c r="F4" s="2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>Email adresini gir</t>
+          <t>Şifre alanına tıkla</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -689,22 +689,18 @@
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>email-input</t>
+          <t>password-input</t>
         </is>
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>Yaz</t>
-        </is>
-      </c>
-      <c r="K4" s="2" t="inlineStr">
-        <is>
-          <t>test@example.com</t>
-        </is>
-      </c>
+          <t>Tıkla</t>
+        </is>
+      </c>
+      <c r="K4" s="2" t="inlineStr"/>
       <c r="L4" s="2" t="inlineStr">
         <is>
-          <t>Email girildi</t>
+          <t>Şifre alanı aktif</t>
         </is>
       </c>
       <c r="M4" s="2" t="inlineStr"/>
@@ -713,17 +709,17 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>TC001</t>
+          <t>TC004</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>Kullanıcı Girişi</t>
+          <t>Giriş Butonu</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Kullanıcının email ve şifre ile giriş yapabilmesi</t>
+          <t>Giriş butonuna tıklanarak giriş yapılması</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
@@ -737,11 +733,11 @@
         </is>
       </c>
       <c r="F5" s="2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>Şifre alanına tıkla</t>
+          <t>Giriş butonuna tıkla</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
@@ -751,7 +747,7 @@
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>password-input</t>
+          <t>login-btn</t>
         </is>
       </c>
       <c r="J5" s="2" t="inlineStr">
@@ -762,7 +758,7 @@
       <c r="K5" s="2" t="inlineStr"/>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>Şifre alanı aktif</t>
+          <t>Giriş yapıldı</t>
         </is>
       </c>
       <c r="M5" s="2" t="inlineStr"/>
@@ -771,22 +767,22 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>TC001</t>
+          <t>TC005</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Kullanıcı Girişi</t>
+          <t>Hatalı Email</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Kullanıcının email ve şifre ile giriş yapabilmesi</t>
+          <t>Geçersiz email ile giriş denemesi</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>Yüksek</t>
+          <t>Orta</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
@@ -795,11 +791,11 @@
         </is>
       </c>
       <c r="F6" s="2" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2" t="inlineStr">
         <is>
-          <t>Şifreyi gir</t>
+          <t>Email alanına geçersiz email gir</t>
         </is>
       </c>
       <c r="H6" s="2" t="inlineStr">
@@ -809,7 +805,7 @@
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>password-input</t>
+          <t>email-input</t>
         </is>
       </c>
       <c r="J6" s="2" t="inlineStr">
@@ -819,12 +815,12 @@
       </c>
       <c r="K6" s="2" t="inlineStr">
         <is>
-          <t>123456</t>
+          <t>invalid@email</t>
         </is>
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>Şifre girildi</t>
+          <t>Hata mesajı görüntülendi</t>
         </is>
       </c>
       <c r="M6" s="2" t="inlineStr"/>
@@ -833,22 +829,22 @@
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>TC001</t>
+          <t>TC006</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>Kullanıcı Girişi</t>
+          <t>Hatalı Şifre</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Kullanıcının email ve şifre ile giriş yapabilmesi</t>
+          <t>Geçersiz şifre ile giriş denemesi</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>Yüksek</t>
+          <t>Orta</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
@@ -857,11 +853,11 @@
         </is>
       </c>
       <c r="F7" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Giriş butonuna tıkla</t>
+          <t>Şifre alanına geçersiz şifre gir</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -871,18 +867,22 @@
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>login-btn</t>
+          <t>password-input</t>
         </is>
       </c>
       <c r="J7" s="2" t="inlineStr">
         <is>
-          <t>Tıkla</t>
-        </is>
-      </c>
-      <c r="K7" s="2" t="inlineStr"/>
+          <t>Yaz</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>wrongpass</t>
+        </is>
+      </c>
       <c r="L7" s="2" t="inlineStr">
         <is>
-          <t>Giriş yapıldı</t>
+          <t>Hata mesajı görüntülendi</t>
         </is>
       </c>
       <c r="M7" s="2" t="inlineStr"/>

</xml_diff>